<commit_message>
fix bug in time computing, solve insonsistence in Greedy
</commit_message>
<xml_diff>
--- a/Delay Model/OutPut/3rd/main_30_1.xlsx
+++ b/Delay Model/OutPut/3rd/main_30_1.xlsx
@@ -49,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -334,7 +335,7 @@
   <dimension ref="A1:AQ10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -343,11 +344,11 @@
       <c r="A1">
         <v>10</v>
       </c>
-      <c r="B1">
-        <v>1007.7017031832961</v>
+      <c r="B1" s="1">
+        <v>1003.59505890593</v>
       </c>
       <c r="C1">
-        <v>11.610091984225621</v>
+        <v>9.8443438331496207</v>
       </c>
       <c r="D1">
         <v>0</v>
@@ -359,7 +360,7 @@
         <v>620.3069828685567</v>
       </c>
       <c r="G1">
-        <v>11.609963455797823</v>
+        <v>9.8418471971860697</v>
       </c>
       <c r="H1">
         <v>0</v>
@@ -389,7 +390,7 @@
         <v>0</v>
       </c>
       <c r="Q1">
-        <v>11.320929594443806</v>
+        <v>9.8584060415702996</v>
       </c>
       <c r="R1">
         <v>0</v>
@@ -398,10 +399,10 @@
         <v>0</v>
       </c>
       <c r="T1">
-        <v>0.10088880917427423</v>
+        <v>0.168095472122096</v>
       </c>
       <c r="U1">
-        <v>11.482808710358334</v>
+        <v>9.9381617420716495</v>
       </c>
       <c r="V1">
         <v>0</v>
@@ -431,7 +432,7 @@
         <v>0</v>
       </c>
       <c r="AE1">
-        <v>11.40305300985715</v>
+        <v>9.8584060415702996</v>
       </c>
       <c r="AF1">
         <v>0</v>
@@ -443,7 +444,7 @@
         <v>8.5346247627656187</v>
       </c>
       <c r="AI1">
-        <v>11.482808710358334</v>
+        <v>9.8621617420716507</v>
       </c>
       <c r="AJ1">
         <v>0</v>
@@ -452,7 +453,7 @@
         <v>0</v>
       </c>
       <c r="AL1">
-        <v>6.5013183859196984</v>
+        <v>5.3002636771839402</v>
       </c>
       <c r="AM1">
         <v>0</v>
@@ -464,7 +465,7 @@
         <v>11.594111135517128</v>
       </c>
       <c r="AP1">
-        <v>6.5013183859197889</v>
+        <v>5.3002636771839402</v>
       </c>
       <c r="AQ1">
         <v>0</v>
@@ -475,10 +476,10 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>2015.4034063665922</v>
+        <v>2007.19</v>
       </c>
       <c r="C2">
-        <v>23.306888923970405</v>
+        <v>19.762205894692976</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -490,7 +491,7 @@
         <v>14347.754780638197</v>
       </c>
       <c r="G2">
-        <v>23.33803678478963</v>
+        <v>19.783816959691134</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -520,22 +521,22 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>36.345545494325229</v>
+        <v>20.246913780813198</v>
       </c>
       <c r="R2">
-        <v>13.215253399716669</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.17962691980095224</v>
+        <v>0.30621881977772297</v>
       </c>
       <c r="U2">
-        <v>36.571095379980427</v>
+        <v>20.243668575374901</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <v>0</v>
@@ -562,7 +563,7 @@
         <v>0</v>
       </c>
       <c r="AE2">
-        <v>23.526064970771657</v>
+        <v>20.246913780813198</v>
       </c>
       <c r="AF2">
         <v>0</v>
@@ -574,7 +575,7 @@
         <v>38.952567741181042</v>
       </c>
       <c r="AI2">
-        <v>23.544566179701238</v>
+        <v>20.142668575374898</v>
       </c>
       <c r="AJ2">
         <v>0</v>
@@ -583,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="AL2">
-        <v>12.147499786197514</v>
+        <v>9.9033685267321747</v>
       </c>
       <c r="AM2">
         <v>0</v>
@@ -595,7 +596,7 @@
         <v>14401.209962895831</v>
       </c>
       <c r="AP2">
-        <v>12.14749978619742</v>
+        <v>9.9033685267321747</v>
       </c>
       <c r="AQ2">
         <v>0</v>
@@ -606,10 +607,10 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>3023.1051095498883</v>
+        <v>3010.7849999999999</v>
       </c>
       <c r="C3">
-        <v>34.338410134882388</v>
+        <v>29.115972251621969</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -621,7 +622,7 @@
         <v>14401.482069347501</v>
       </c>
       <c r="G3">
-        <v>34.381989785775879</v>
+        <v>29.145853136844799</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -651,22 +652,22 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>54.249526950404587</v>
+        <v>33.6820803978732</v>
       </c>
       <c r="R3">
-        <v>19.839673605178888</v>
+        <v>3.6005505040752901</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>0.28943463550843612</v>
+        <v>0.25953717764963702</v>
       </c>
       <c r="U3">
-        <v>54.592395590439097</v>
+        <v>33.5153119842563</v>
       </c>
       <c r="V3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -693,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="AE3">
-        <v>38.296703146829145</v>
+        <v>29.971552574152799</v>
       </c>
       <c r="AF3">
         <v>0</v>
@@ -705,7 +706,7 @@
         <v>64.125815604293848</v>
       </c>
       <c r="AI3">
-        <v>38.459458116224283</v>
+        <v>29.830050650016101</v>
       </c>
       <c r="AJ3">
         <v>0</v>
@@ -714,7 +715,7 @@
         <v>0</v>
       </c>
       <c r="AL3">
-        <v>15.219152418468077</v>
+        <v>12.407563508323898</v>
       </c>
       <c r="AM3">
         <v>0</v>
@@ -726,7 +727,7 @@
         <v>14401.147309315706</v>
       </c>
       <c r="AP3">
-        <v>15.219152418467756</v>
+        <v>12.407563508323898</v>
       </c>
       <c r="AQ3">
         <v>0</v>
@@ -737,10 +738,10 @@
         <v>40</v>
       </c>
       <c r="B4">
-        <v>4030.8068127331844</v>
+        <v>4014.3802356237202</v>
       </c>
       <c r="C4">
-        <v>49.444886594813646</v>
+        <v>41.924944702572205</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -752,7 +753,7 @@
         <v>14401.561931407856</v>
       </c>
       <c r="G4">
-        <v>49.449597484429084</v>
+        <v>41.918769534202987</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -782,22 +783,22 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>66.625112536353555</v>
+        <v>44.5139527215917</v>
       </c>
       <c r="R4">
-        <v>19.854092849250854</v>
+        <v>3.60279407845462</v>
       </c>
       <c r="S4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T4">
-        <v>0.36029285112663617</v>
+        <v>0.55463936423556404</v>
       </c>
       <c r="U4">
-        <v>67.9296013986513</v>
+        <v>44.492482389639697</v>
       </c>
       <c r="V4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W4">
         <v>0</v>
@@ -824,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="AE4">
-        <v>48.380350626176032</v>
+        <v>40.579156675758099</v>
       </c>
       <c r="AF4">
         <v>0</v>
@@ -836,7 +837,7 @@
         <v>63.700353026881558</v>
       </c>
       <c r="AI4">
-        <v>48.251998331694928</v>
+        <v>40.389720018337499</v>
       </c>
       <c r="AJ4">
         <v>0</v>
@@ -845,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="AL4">
-        <v>20.681192778312155</v>
+        <v>16.860545565823742</v>
       </c>
       <c r="AM4">
         <v>0</v>
@@ -857,7 +858,7 @@
         <v>14401.377711899091</v>
       </c>
       <c r="AP4">
-        <v>20.681192778312539</v>
+        <v>16.860545565823742</v>
       </c>
       <c r="AQ4">
         <v>0</v>
@@ -868,10 +869,10 @@
         <v>50</v>
       </c>
       <c r="B5">
-        <v>5038.508515916481</v>
+        <v>5017.9750000000004</v>
       </c>
       <c r="C5">
-        <v>62.288166680273626</v>
+        <v>52.814924323620332</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -883,7 +884,7 @@
         <v>14401.561931407856</v>
       </c>
       <c r="G5">
-        <v>62.242600698812552</v>
+        <v>52.763487806438086</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -913,22 +914,22 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>85.892669335233776</v>
+        <v>59.013022503787198</v>
       </c>
       <c r="R5">
-        <v>26.485551825206777</v>
+        <v>7.2063673323367903</v>
       </c>
       <c r="S5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T5">
-        <v>0.507800092602396</v>
+        <v>0.47483142729368699</v>
       </c>
       <c r="U5">
-        <v>89.580643668510149</v>
+        <v>58.896324587335798</v>
       </c>
       <c r="V5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -955,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="AE5">
-        <v>71.609225586650368</v>
+        <v>51.806655171450416</v>
       </c>
       <c r="AF5">
         <v>0</v>
@@ -967,7 +968,7 @@
         <v>89.995868052647467</v>
       </c>
       <c r="AI5">
-        <v>71.805229232584878</v>
+        <v>51.63602472628682</v>
       </c>
       <c r="AJ5">
         <v>0</v>
@@ -976,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="AL5">
-        <v>24.923966490079255</v>
+        <v>20.319508511507696</v>
       </c>
       <c r="AM5">
         <v>0</v>
@@ -988,7 +989,7 @@
         <v>14401.15026160967</v>
       </c>
       <c r="AP5">
-        <v>24.923394210603647</v>
+        <v>20.319508511507696</v>
       </c>
       <c r="AQ5">
         <v>0</v>
@@ -999,10 +1000,10 @@
         <v>60</v>
       </c>
       <c r="B6">
-        <v>6046.2102190997766</v>
+        <v>6021.57</v>
       </c>
       <c r="C6">
-        <v>78.359282190508296</v>
+        <v>66.441826425685477</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1014,7 +1015,7 @@
         <v>14401.561931407856</v>
       </c>
       <c r="G6">
-        <v>77.52951757761366</v>
+        <v>65.722314129195553</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1044,22 +1045,22 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>111.23808984513201</v>
+        <v>72.739582554584601</v>
       </c>
       <c r="R6">
-        <v>39.743009145469316</v>
+        <v>10.8113858788711</v>
       </c>
       <c r="S6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T6">
-        <v>0.56654967581260185</v>
+        <v>0.81762305768054699</v>
       </c>
       <c r="U6">
-        <v>118.25529877868419</v>
+        <v>72.736482035728102</v>
       </c>
       <c r="V6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -1086,7 +1087,7 @@
         <v>0</v>
       </c>
       <c r="AE6">
-        <v>81.523672506502834</v>
+        <v>63.58193729589297</v>
       </c>
       <c r="AF6">
         <v>0</v>
@@ -1098,7 +1099,7 @@
         <v>89.204979196065821</v>
       </c>
       <c r="AI6">
-        <v>81.47986147495763</v>
+        <v>63.309559718920667</v>
       </c>
       <c r="AJ6">
         <v>0</v>
@@ -1107,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="AL6">
-        <v>29.022875724300228</v>
+        <v>23.661184528677854</v>
       </c>
       <c r="AM6">
         <v>0</v>
@@ -1119,7 +1120,7 @@
         <v>14401.15026160967</v>
       </c>
       <c r="AP6">
-        <v>29.02218482651859</v>
+        <v>23.661184528677854</v>
       </c>
       <c r="AQ6">
         <v>0</v>
@@ -1130,10 +1131,10 @@
         <v>70</v>
       </c>
       <c r="B7">
-        <v>7053.9119222830723</v>
+        <v>7025.165</v>
       </c>
       <c r="C7">
-        <v>90.518730630274703</v>
+        <v>76.751976545525295</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1145,7 +1146,7 @@
         <v>14401.561931407856</v>
       </c>
       <c r="G7">
-        <v>88.670626387976526</v>
+        <v>75.166709965261504</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1175,22 +1176,22 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>129.3999864619901</v>
+        <v>86.239626855793304</v>
       </c>
       <c r="R7">
-        <v>46.413741050287996</v>
+        <v>14.429689694999899</v>
       </c>
       <c r="S7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="T7">
-        <v>0.74274390696777726</v>
+        <v>0.67079966751631204</v>
       </c>
       <c r="U7">
-        <v>143.15571560736009</v>
+        <v>85.936981971805906</v>
       </c>
       <c r="V7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -1217,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="AE7">
-        <v>97.090480951759844</v>
+        <v>71.275137071940804</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -1229,7 +1230,7 @@
         <v>124.62845500961579</v>
       </c>
       <c r="AI7">
-        <v>97.034259425457293</v>
+        <v>71.08841213164861</v>
       </c>
       <c r="AJ7">
         <v>0</v>
@@ -1238,7 +1239,7 @@
         <v>0</v>
       </c>
       <c r="AL7">
-        <v>33.341919853208267</v>
+        <v>27.182327681147452</v>
       </c>
       <c r="AM7">
         <v>0</v>
@@ -1250,7 +1251,7 @@
         <v>14401.15026160967</v>
       </c>
       <c r="AP7">
-        <v>33.341670299544944</v>
+        <v>27.182327681147452</v>
       </c>
       <c r="AQ7">
         <v>0</v>
@@ -1261,10 +1262,10 @@
         <v>80</v>
       </c>
       <c r="B8">
-        <v>8061.6136254663688</v>
+        <v>8028.76</v>
       </c>
       <c r="C8">
-        <v>106.71900243095779</v>
+        <v>90.488391899777923</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1276,7 +1277,7 @@
         <v>14401.561931407856</v>
       </c>
       <c r="G8">
-        <v>105.67266658757552</v>
+        <v>89.579458319030508</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1306,22 +1307,22 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>149.30863478946316</v>
+        <v>97.670613402044097</v>
       </c>
       <c r="R8">
-        <v>53.067390036394642</v>
+        <v>14.437213776425301</v>
       </c>
       <c r="S8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="T8">
-        <v>0.84094945900289664</v>
+        <v>0.76349608810185599</v>
       </c>
       <c r="U8">
-        <v>172.40835467639823</v>
+        <v>97.605318861791702</v>
       </c>
       <c r="V8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="W8">
         <v>0</v>
@@ -1348,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="AE8">
-        <v>127.20223974940225</v>
+        <v>83.233399625618802</v>
       </c>
       <c r="AF8">
         <v>0</v>
@@ -1360,7 +1361,7 @@
         <v>133.77285153750003</v>
       </c>
       <c r="AI8">
-        <v>127.43112114571169</v>
+        <v>82.751206203536711</v>
       </c>
       <c r="AJ8">
         <v>0</v>
@@ -1369,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="AL8">
-        <v>42.782384635737827</v>
+        <v>34.878759329679497</v>
       </c>
       <c r="AM8">
         <v>0</v>
@@ -1381,7 +1382,7 @@
         <v>14401.15026160967</v>
       </c>
       <c r="AP8">
-        <v>42.781740235582689</v>
+        <v>34.878759329679497</v>
       </c>
       <c r="AQ8">
         <v>0</v>
@@ -1392,10 +1393,10 @@
         <v>90</v>
       </c>
       <c r="B9">
-        <v>9069.3153286496654</v>
+        <v>9032.3549999999996</v>
       </c>
       <c r="C9">
-        <v>115.30387635914404</v>
+        <v>97.767615081483342</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1407,7 +1408,7 @@
         <v>14401.561931407856</v>
       </c>
       <c r="G9">
-        <v>113.26548352404919</v>
+        <v>96.015942324297782</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1437,22 +1438,22 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>174.97496432892825</v>
+        <v>124.115303890785</v>
       </c>
       <c r="R9">
-        <v>59.765409987693829</v>
+        <v>18.064179306943402</v>
       </c>
       <c r="S9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="T9">
-        <v>0.94514888284532717</v>
+        <v>0.77696965770298698</v>
       </c>
       <c r="U9">
-        <v>255.45700046795636</v>
+        <v>123.67664374211</v>
       </c>
       <c r="V9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="W9">
         <v>0</v>
@@ -1479,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="AE9">
-        <v>177.31834750517655</v>
+        <v>95.656717140325796</v>
       </c>
       <c r="AF9">
         <v>0</v>
@@ -1491,7 +1492,7 @@
         <v>110.9318989180058</v>
       </c>
       <c r="AI9">
-        <v>177.13029483547257</v>
+        <v>96.109047046121802</v>
       </c>
       <c r="AJ9">
         <v>0</v>
@@ -1500,7 +1501,7 @@
         <v>0</v>
       </c>
       <c r="AL9">
-        <v>51.55801778768857</v>
+        <v>42.033180460678423</v>
       </c>
       <c r="AM9">
         <v>0</v>
@@ -1512,7 +1513,7 @@
         <v>14401.15026160967</v>
       </c>
       <c r="AP9">
-        <v>51.557286290819604</v>
+        <v>42.033180460678423</v>
       </c>
       <c r="AQ9">
         <v>0</v>
@@ -1523,10 +1524,10 @@
         <v>100</v>
       </c>
       <c r="B10">
-        <v>10077.017031832962</v>
+        <v>10035.950000000001</v>
       </c>
       <c r="C10">
-        <v>129.14182065652199</v>
+        <v>109.5009830679254</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1538,7 +1539,7 @@
         <v>14401.561931407856</v>
       </c>
       <c r="G10">
-        <v>128.01058372119942</v>
+        <v>108.51546685769162</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1568,22 +1569,22 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>240.14177056131749</v>
+        <v>391.97301839833398</v>
       </c>
       <c r="R10">
-        <v>66.428255407876549</v>
+        <v>21.6745402885741</v>
       </c>
       <c r="S10">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="T10">
-        <v>0.86559378520984875</v>
+        <v>0.691298614282576</v>
       </c>
       <c r="U10">
-        <v>1543.3087425239835</v>
+        <v>392.11048864042999</v>
       </c>
       <c r="V10">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -1610,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="AE10">
-        <v>188.62267503091516</v>
+        <v>172.62497268322946</v>
       </c>
       <c r="AF10">
         <v>0</v>
@@ -1622,7 +1623,7 @@
         <v>170.41402317904343</v>
       </c>
       <c r="AI10">
-        <v>189.05947933462915</v>
+        <v>172.75331597934044</v>
       </c>
       <c r="AJ10">
         <v>0</v>
@@ -1631,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="AL10">
-        <v>60.036967117524334</v>
+        <v>48.945727191344986</v>
       </c>
       <c r="AM10">
         <v>0</v>
@@ -1643,7 +1644,7 @@
         <v>14401.15026160967</v>
       </c>
       <c r="AP10">
-        <v>60.036168398335462</v>
+        <v>48.945727191344986</v>
       </c>
       <c r="AQ10">
         <v>0</v>
@@ -1651,5 +1652,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>